<commit_message>
Überarbeiten und WIR-Teil nach Vorlage beginnen
</commit_message>
<xml_diff>
--- a/form/WIR-Teil.xlsx
+++ b/form/WIR-Teil.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -117,17 +117,84 @@
   </si>
   <si>
     <t>Elektrolyt-Kondensatoren</t>
+  </si>
+  <si>
+    <t>Hardwareentwicklung</t>
+  </si>
+  <si>
+    <t>Optimierungsarbeiten</t>
+  </si>
+  <si>
+    <t>Messungen</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Gesamtarbeitszeit</t>
+  </si>
+  <si>
+    <t>Stundenlohn (Techniker)</t>
+  </si>
+  <si>
+    <t>Entwicklungskosten</t>
+  </si>
+  <si>
+    <t>Bürofläche für 2 Personen</t>
+  </si>
+  <si>
+    <t>monatliche Miete</t>
+  </si>
+  <si>
+    <t>Dauer des Mietverhältnisses</t>
+  </si>
+  <si>
+    <t>Gesamtmietkosten</t>
+  </si>
+  <si>
+    <t>Wasser</t>
+  </si>
+  <si>
+    <t>Heizung</t>
+  </si>
+  <si>
+    <t>Strom</t>
+  </si>
+  <si>
+    <t>Internet &amp; Telefon</t>
+  </si>
+  <si>
+    <t>Gesamtkosten</t>
+  </si>
+  <si>
+    <t>Betriebskosten</t>
+  </si>
+  <si>
+    <t>Gesamtentwicklungskosten</t>
+  </si>
+  <si>
+    <t>Gesamtbetriebskosten</t>
+  </si>
+  <si>
+    <t>Fixkosten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="0.000&quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="0&quot; h&quot;"/>
+    <numFmt numFmtId="167" formatCode="0&quot; m²&quot;"/>
+    <numFmt numFmtId="169" formatCode="0&quot; Monate&quot;"/>
+    <numFmt numFmtId="171" formatCode="0&quot; € / Monat&quot;"/>
+    <numFmt numFmtId="172" formatCode="0&quot; € / m²&quot;"/>
+    <numFmt numFmtId="175" formatCode="#&quot;.&quot;##0.00&quot; €&quot;"/>
+    <numFmt numFmtId="176" formatCode="##0.00&quot; €&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +210,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -212,55 +287,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,10 +414,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,10 +421,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -290,9 +428,125 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,497 +862,830 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E1" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="6" width="10.77734375" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="G1" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.68</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>2+2</f>
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="27">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <f>D2*$E$2</f>
         <v>0.41199999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2">
+      <c r="G2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="42">
+        <v>230</v>
+      </c>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3">
+      <c r="C3" s="25"/>
+      <c r="D3" s="2">
         <f>1+1+1+1</f>
         <v>4</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5">
+      <c r="E3" s="27"/>
+      <c r="F3" s="3">
         <f t="shared" ref="F3:F16" si="0">D3*$E$2</f>
         <v>0.41199999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2">
+      <c r="G3" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="42">
+        <v>80</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="1">
         <v>10</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3">
+      <c r="C4" s="25"/>
+      <c r="D4" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5">
+      <c r="E4" s="27"/>
+      <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>0.10299999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2">
+      <c r="G4" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="42">
+        <v>60</v>
+      </c>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
+      <c r="B5" s="1">
         <v>100</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3">
+      <c r="C5" s="25"/>
+      <c r="D5" s="2">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5">
+      <c r="E5" s="27"/>
+      <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>0.61799999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2">
+      <c r="G5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="43">
+        <v>70</v>
+      </c>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="1">
         <v>330</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3">
+      <c r="C6" s="25"/>
+      <c r="D6" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5">
+      <c r="E6" s="27"/>
+      <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>0.10299999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2">
+      <c r="G6" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="44">
+        <f>SUM(K2:M5)</f>
+        <v>440</v>
+      </c>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="1">
         <v>560</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3">
+      <c r="C7" s="25"/>
+      <c r="D7" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5">
+      <c r="E7" s="27"/>
+      <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>0.10299999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="G7" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="45">
+        <v>100</v>
+      </c>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3">
+      <c r="C8" s="25"/>
+      <c r="D8" s="2">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5">
+      <c r="E8" s="27"/>
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+      <c r="G8" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="52">
+        <f>K6*K7</f>
+        <v>44000</v>
+      </c>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3">
+      <c r="C9" s="25"/>
+      <c r="D9" s="2">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5">
+      <c r="E9" s="27"/>
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3">
+      <c r="C10" s="25"/>
+      <c r="D10" s="2">
         <f>3+2+1+1</f>
         <v>7</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5">
+      <c r="E10" s="27"/>
+      <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3">
+      <c r="C11" s="25"/>
+      <c r="D11" s="2">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5">
+      <c r="E11" s="27"/>
+      <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="G11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3">
+      <c r="C12" s="25"/>
+      <c r="D12" s="2">
         <f>2+6</f>
         <v>8</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5">
+      <c r="E12" s="27"/>
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0.82399999999999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="G12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="47">
+        <v>20</v>
+      </c>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3">
+      <c r="C13" s="25"/>
+      <c r="D13" s="2">
         <f>2+2</f>
         <v>4</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5">
+      <c r="E13" s="27"/>
+      <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0.41199999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+      <c r="G13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="49">
+        <v>5</v>
+      </c>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3">
+      <c r="C14" s="25"/>
+      <c r="D14" s="2">
         <f>3+4+3+3+4+2</f>
         <v>19</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5">
+      <c r="E14" s="27"/>
+      <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>1.9569999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="G14" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="50">
+        <v>9</v>
+      </c>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3">
+      <c r="C15" s="25"/>
+      <c r="D15" s="2">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5">
+      <c r="E15" s="27"/>
+      <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
+      <c r="G15" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="55">
+        <f>K14*K13*K12</f>
+        <v>900</v>
+      </c>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="8">
+      <c r="C16" s="26"/>
+      <c r="D16" s="5">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="5">
+      <c r="E16" s="28"/>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="7">
         <v>1</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="29">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="8">
         <f>D17*$E$17</f>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
+      <c r="G17" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="48">
+        <v>25</v>
+      </c>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3">
+      <c r="C18" s="25"/>
+      <c r="D18" s="2">
         <f>4</f>
         <v>4</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16">
+      <c r="E18" s="30"/>
+      <c r="F18" s="9">
         <f t="shared" ref="F18:F23" si="1">D18*$E$17</f>
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="G18" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="48">
+        <v>85</v>
+      </c>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="3">
+      <c r="C19" s="25"/>
+      <c r="D19" s="2">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16">
+      <c r="E19" s="30"/>
+      <c r="F19" s="9">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+      <c r="G19" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="48">
+        <v>50</v>
+      </c>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3">
+      <c r="C20" s="25"/>
+      <c r="D20" s="2">
         <f>1+1+1+1+1+5</f>
         <v>10</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16">
+      <c r="E20" s="30"/>
+      <c r="F20" s="9">
         <f t="shared" si="1"/>
         <v>1.4000000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
+      <c r="G20" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="51">
+        <v>40</v>
+      </c>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="3">
+      <c r="C21" s="25"/>
+      <c r="D21" s="2">
         <f>1+1+1+1</f>
         <v>4</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16">
+      <c r="E21" s="30"/>
+      <c r="F21" s="9">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
+      <c r="G21" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="52">
+        <f>(K17+K18+K19+K20)*K14</f>
+        <v>1800</v>
+      </c>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3">
+      <c r="C22" s="25"/>
+      <c r="D22" s="2">
         <f>3+3</f>
         <v>6</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16">
+      <c r="E22" s="30"/>
+      <c r="F22" s="9">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="8">
+      <c r="C23" s="26"/>
+      <c r="D23" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18">
+      <c r="E23" s="31"/>
+      <c r="F23" s="10">
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="G23" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="52">
+        <f>K15+K21</f>
+        <v>2700</v>
+      </c>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="12">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="13">
         <v>0.15</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="53">
         <f>D24*E24</f>
         <v>0.15</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25" t="s">
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="26">
+      <c r="C25" s="25"/>
+      <c r="D25" s="15">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="16">
         <v>0.09</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="54">
         <f t="shared" ref="F25:F28" si="2">D25*E25</f>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25" t="s">
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="26">
+      <c r="C26" s="25"/>
+      <c r="D26" s="15">
         <f>7+3+3+4</f>
         <v>17</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="16">
         <v>0.08</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="54">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25" t="s">
+      <c r="G26" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="26">
+      <c r="C27" s="25"/>
+      <c r="D27" s="15">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="16">
         <v>0.09</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="54">
         <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30" t="s">
+      <c r="G27" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="60">
+        <f>K8</f>
+        <v>44000</v>
+      </c>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23"/>
+      <c r="B28" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="31">
+      <c r="C28" s="26"/>
+      <c r="D28" s="18">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="19">
         <v>1.6</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="59">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
+      <c r="G28" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="61">
+        <f>K23</f>
+        <v>2700</v>
+      </c>
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="52">
+        <f>K27+K28</f>
+        <v>46700</v>
+      </c>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="55">
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="G11:M11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="C24:C28"/>
     <mergeCell ref="A2:A16"/>

</xml_diff>

<commit_message>
Arbeitsnachweis (form) & kleinere Anpassungen
</commit_message>
<xml_diff>
--- a/form/WIR-Teil.xlsx
+++ b/form/WIR-Teil.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -188,11 +188,11 @@
     <numFmt numFmtId="165" formatCode="0.000&quot;€&quot;"/>
     <numFmt numFmtId="166" formatCode="0&quot; h&quot;"/>
     <numFmt numFmtId="167" formatCode="0&quot; m²&quot;"/>
-    <numFmt numFmtId="169" formatCode="0&quot; Monate&quot;"/>
-    <numFmt numFmtId="171" formatCode="0&quot; € / Monat&quot;"/>
-    <numFmt numFmtId="172" formatCode="0&quot; € / m²&quot;"/>
-    <numFmt numFmtId="175" formatCode="#&quot;.&quot;##0.00&quot; €&quot;"/>
-    <numFmt numFmtId="176" formatCode="##0.00&quot; €&quot;"/>
+    <numFmt numFmtId="168" formatCode="0&quot; Monate&quot;"/>
+    <numFmt numFmtId="169" formatCode="0&quot; € / Monat&quot;"/>
+    <numFmt numFmtId="170" formatCode="0&quot; € / m²&quot;"/>
+    <numFmt numFmtId="171" formatCode="#&quot;.&quot;##0.00&quot; €&quot;"/>
+    <numFmt numFmtId="172" formatCode="##0.00&quot; €&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -227,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -291,15 +291,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -364,23 +355,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -389,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,6 +413,87 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -464,90 +527,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -864,18 +855,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E1" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -894,602 +885,602 @@
       <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>0.68</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="52" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="2">
         <f>2+2</f>
         <v>4</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="54">
         <v>0.10299999999999999</v>
       </c>
       <c r="F2" s="3">
         <f>D2*$E$2</f>
         <v>0.41199999999999998</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="42">
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="38">
         <v>230</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="2">
         <f>1+1+1+1</f>
         <v>4</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F16" si="0">D3*$E$2</f>
         <v>0.41199999999999998</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="42">
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="38">
         <v>80</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="52"/>
       <c r="B4" s="1">
         <v>10</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>0.10299999999999999</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="42">
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="38">
         <v>60</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
       <c r="B5" s="1">
         <v>100</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="2">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>0.61799999999999999</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="43">
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="42">
         <v>70</v>
       </c>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="52"/>
       <c r="B6" s="1">
         <v>330</v>
       </c>
-      <c r="C6" s="25"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>0.10299999999999999</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="44">
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="43">
         <f>SUM(K2:M5)</f>
         <v>440</v>
       </c>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="52"/>
       <c r="B7" s="1">
         <v>560</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>0.10299999999999999</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="45">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="44">
         <v>100</v>
       </c>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="2">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E8" s="27"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="52">
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24">
         <f>K6*K7</f>
         <v>44000</v>
       </c>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="2">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E9" s="27"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="2">
         <f>3+2+1+1</f>
         <v>7</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>0.72099999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="2">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E11" s="27"/>
+      <c r="E11" s="54"/>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="41"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="2">
         <f>2+6</f>
         <v>8</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>0.82399999999999995</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="47">
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="39">
         <v>20</v>
       </c>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="52"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="2">
         <f>2+2</f>
         <v>4</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>0.41199999999999998</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="49">
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="40">
         <v>5</v>
       </c>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="52"/>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="2">
         <f>3+4+3+3+4+2</f>
         <v>19</v>
       </c>
-      <c r="E14" s="27"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>1.9569999999999999</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="50">
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="36">
         <v>9</v>
       </c>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="52"/>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="2">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="55">
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="37">
         <f>K14*K13*K12</f>
         <v>900</v>
       </c>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="53"/>
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="5">
         <f>2</f>
         <v>2</v>
       </c>
-      <c r="E16" s="28"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="51" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="51" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="56">
         <v>0.14000000000000001</v>
       </c>
       <c r="F17" s="8">
         <f>D17*$E$17</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="48">
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="35">
         <v>25</v>
       </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="52"/>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="2">
         <f>4</f>
         <v>4</v>
       </c>
-      <c r="E18" s="30"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="9">
         <f t="shared" ref="F18:F23" si="1">D18*$E$17</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="48">
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="35">
         <v>85</v>
       </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="52"/>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="2">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="E19" s="30"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="9">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="48">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="35">
         <v>50</v>
       </c>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="52"/>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="2">
         <f>1+1+1+1+1+5</f>
         <v>10</v>
       </c>
-      <c r="E20" s="30"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="9">
         <f t="shared" si="1"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="51">
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="33">
         <v>40</v>
       </c>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="2">
         <f>1+1+1+1</f>
         <v>4</v>
       </c>
-      <c r="E21" s="30"/>
+      <c r="E21" s="57"/>
       <c r="F21" s="9">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="52">
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24">
         <f>(K17+K18+K19+K20)*K14</f>
         <v>1800</v>
       </c>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="52"/>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="2">
         <f>3+3</f>
         <v>6</v>
       </c>
-      <c r="E22" s="30"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="9">
         <f t="shared" si="1"/>
         <v>0.84000000000000008</v>
       </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53"/>
       <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="5">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E23" s="31"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="10">
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="52">
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24">
         <f>K15+K21</f>
         <v>2700</v>
       </c>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="51" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="12">
@@ -1499,24 +1490,24 @@
       <c r="E24" s="13">
         <v>0.15</v>
       </c>
-      <c r="F24" s="53">
+      <c r="F24" s="62">
         <f>D24*E24</f>
         <v>0.15</v>
       </c>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="49"/>
       <c r="B25" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="25"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="15">
         <f>1+1</f>
         <v>2</v>
@@ -1524,24 +1515,24 @@
       <c r="E25" s="16">
         <v>0.09</v>
       </c>
-      <c r="F25" s="54">
+      <c r="F25" s="63">
         <f t="shared" ref="F25:F28" si="2">D25*E25</f>
         <v>0.18</v>
       </c>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
       <c r="B26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="25"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="15">
         <f>7+3+3+4</f>
         <v>17</v>
@@ -1549,26 +1540,26 @@
       <c r="E26" s="16">
         <v>0.08</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F26" s="63">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G26" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="41"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="27"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
       <c r="B27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="25"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="15">
         <f>1+1</f>
         <v>2</v>
@@ -1576,29 +1567,29 @@
       <c r="E27" s="16">
         <v>0.09</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="63">
         <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G27" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="60">
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="29">
         <f>K8</f>
         <v>44000</v>
       </c>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="50"/>
       <c r="B28" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="18">
         <f>1+1</f>
         <v>2</v>
@@ -1606,82 +1597,39 @@
       <c r="E28" s="19">
         <v>1.6</v>
       </c>
-      <c r="F28" s="59">
+      <c r="F28" s="64">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="61">
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="31">
         <f>K23</f>
         <v>2700</v>
       </c>
-      <c r="L28" s="61"/>
-      <c r="M28" s="61"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="37" t="s">
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="52">
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24">
         <f>K27+K28</f>
         <v>46700</v>
       </c>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="G26:M26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="G11:M11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G3:J3"/>
@@ -1694,6 +1642,49 @@
     <mergeCell ref="C17:C23"/>
     <mergeCell ref="A17:A23"/>
     <mergeCell ref="E17:E23"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="G11:M11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:M28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>